<commit_message>
code for updating format in report_ca_nha
</commit_message>
<xml_diff>
--- a/report_ca_nhan/NV-1 Đỗ Tiến Hải 7-2024.xlsx
+++ b/report_ca_nhan/NV-1 Đỗ Tiến Hải 7-2024.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,6 +528,44 @@
           <t>Phụ phẫu 2</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v/>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>